<commit_message>
[server] Add: daily updated ticket search keywords
</commit_message>
<xml_diff>
--- a/source/server/block_list.xlsx
+++ b/source/server/block_list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2020" yWindow="0" windowWidth="20500" windowHeight="7760" tabRatio="146"/>
+    <workbookView xWindow="9780" yWindow="1040" windowWidth="25600" windowHeight="16060" tabRatio="146"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
   <si>
     <t>weibo</t>
   </si>
@@ -159,13 +159,64 @@
   <si>
     <t>UCNEST</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>每天都是五月病</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>yeezyyu</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>英城置业</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>6aptcom</t>
+  </si>
+  <si>
+    <t>家1号Homplus</t>
+  </si>
+  <si>
+    <t>睿知-伦敦生活服务管家</t>
+  </si>
+  <si>
+    <t>涌正投资_英国置业一站式服务</t>
+  </si>
+  <si>
+    <t>thechampsuk</t>
+  </si>
+  <si>
+    <t>reesekhe</t>
+  </si>
+  <si>
+    <t>qhdy</t>
+  </si>
+  <si>
+    <t>LondonFunHome</t>
+  </si>
+  <si>
+    <t>异乡好居-英国</t>
+  </si>
+  <si>
+    <t>优辰公寓</t>
+  </si>
+  <si>
+    <t>异乡好居--北美</t>
+  </si>
+  <si>
+    <t>键川居-英国</t>
+  </si>
+  <si>
+    <t>异乡好居-新西兰</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -214,6 +265,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="37.4"/>
+      <color rgb="FF000000"/>
+      <name val="SimSun"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -255,7 +312,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -270,6 +327,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -623,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="340" zoomScaleNormal="340" zoomScalePageLayoutView="340" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A19" sqref="A19:A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -794,10 +854,76 @@
       <c r="A13" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="14">
+      <c r="C13" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="42">
       <c r="A14" s="1" t="s">
         <v>43</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="14">
+      <c r="A15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="14">
+      <c r="A16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="14">
+      <c r="A17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14">
+      <c r="A18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14">
+      <c r="A19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14">
+      <c r="A20" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14">
+      <c r="A21" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14">
+      <c r="A22" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14">
+      <c r="A23" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[server] Mod: update libfelix
</commit_message>
<xml_diff>
--- a/source/server/block_list.xlsx
+++ b/source/server/block_list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9780" yWindow="1040" windowWidth="25600" windowHeight="16060" tabRatio="146"/>
+    <workbookView xWindow="13000" yWindow="920" windowWidth="25600" windowHeight="16060" tabRatio="146"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="84">
   <si>
     <t>weibo</t>
   </si>
@@ -210,13 +210,93 @@
   </si>
   <si>
     <t>异乡好居-新西兰</t>
+  </si>
+  <si>
+    <t>yaju</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kaden_London</t>
+  </si>
+  <si>
+    <t>Champ0s7</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>luosine</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>洋房東</t>
+  </si>
+  <si>
+    <t>UKCHINA房产中心</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>陈莉--纽约房产经纪人</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>格拉斯哥租房助手</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>考文垂租房我家房产Coventry</t>
+  </si>
+  <si>
+    <t>英城置业</t>
+  </si>
+  <si>
+    <t>英国高乐家地产</t>
+  </si>
+  <si>
+    <t>英国申请小能手</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UKCHINA房产中心</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>陈莉--纽约房产经纪人</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>格拉斯哥租房助手</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>伦敦租房君</t>
+  </si>
+  <si>
+    <t>英国高乐家地产</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>英国申请小能手</t>
+  </si>
+  <si>
+    <t>Danny</t>
+  </si>
+  <si>
+    <t>LONDONPROPERTY</t>
+  </si>
+  <si>
+    <t>uk china max</t>
+  </si>
+  <si>
+    <t>我的豆瓣账号</t>
+  </si>
+  <si>
+    <t>在英伦的Steven</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -271,6 +351,18 @@
       <name val="SimSun"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="17.600000000000001"/>
+      <color rgb="FF000000"/>
+      <name val="SimSun"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="24.55"/>
+      <color rgb="FF000000"/>
+      <name val="SimSun"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -312,7 +404,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -329,6 +421,12 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -683,10 +781,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="340" zoomScaleNormal="340" zoomScalePageLayoutView="340" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:A23"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -841,21 +939,30 @@
       <c r="C11" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="14">
+      <c r="D11">
+        <v>3226</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="42">
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="13">
+      <c r="D12" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="21">
       <c r="A13" s="3" t="s">
         <v>42</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>45</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="42">
@@ -865,6 +972,9 @@
       <c r="C14" s="5" t="s">
         <v>46</v>
       </c>
+      <c r="D14" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="14">
       <c r="A15" s="1" t="s">
@@ -873,6 +983,9 @@
       <c r="C15" s="3" t="s">
         <v>47</v>
       </c>
+      <c r="D15" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="14">
       <c r="A16" s="1" t="s">
@@ -906,24 +1019,126 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="14">
+    <row r="20" spans="1:3" ht="42">
       <c r="A20" s="1" t="s">
         <v>57</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14">
       <c r="A21" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="C21" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="22" spans="1:3" ht="14">
       <c r="A22" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="C22" s="1" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="23" spans="1:3" ht="14">
       <c r="A23" s="1" t="s">
         <v>60</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="21">
+      <c r="A24" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="21">
+      <c r="A25" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14">
+      <c r="A26" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="14">
+      <c r="A27" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="14">
+      <c r="A28" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="14">
+      <c r="A29" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="14">
+      <c r="A30" s="1"/>
+    </row>
+    <row r="31" spans="1:3" ht="13">
+      <c r="A31" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="30">
+      <c r="A32" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="21">
+      <c r="A33" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="13">
+      <c r="A34" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="14">
+      <c r="A35" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="14">
+      <c r="A36" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="14">
+      <c r="A37" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="13">
+      <c r="A38" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="14">
+      <c r="A39" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[server] Mod: update block_list
</commit_message>
<xml_diff>
--- a/source/server/block_list.xlsx
+++ b/source/server/block_list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13000" yWindow="920" windowWidth="25600" windowHeight="16060" tabRatio="146"/>
+    <workbookView xWindow="-27200" yWindow="4140" windowWidth="25600" windowHeight="16060" tabRatio="146"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="88">
   <si>
     <t>weibo</t>
   </si>
@@ -290,13 +290,29 @@
   </si>
   <si>
     <t>在英伦的Steven</t>
+  </si>
+  <si>
+    <t>londonrooms888</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>thechampsuk</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>tonyWang666</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>在英伦的Alina</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -314,12 +330,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="SimSun"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <u/>
       <sz val="10"/>
       <color theme="10"/>
@@ -334,34 +344,11 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="37.4"/>
-      <color rgb="FF000000"/>
       <name val="SimSun"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="17.600000000000001"/>
-      <color rgb="FF000000"/>
-      <name val="SimSun"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="24.55"/>
-      <color rgb="FF000000"/>
-      <name val="SimSun"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -381,63 +368,56 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -784,72 +764,76 @@
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="340" zoomScaleNormal="340" zoomScalePageLayoutView="340" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="16384" width="9" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14">
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14">
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -859,25 +843,25 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="14">
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="14">
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -887,7 +871,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="14">
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
@@ -900,11 +884,11 @@
       <c r="D8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="14">
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
@@ -918,7 +902,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="14">
+    <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -932,62 +916,71 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="14">
+    <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="B11" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="C11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>3226</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="42">
+    <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="B12" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="C12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="21">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:5">
+      <c r="A13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="B13" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="42">
+    <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="1" t="s">
         <v>46</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="14">
+    <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="14">
+    <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
         <v>49</v>
       </c>
@@ -995,7 +988,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="14">
+    <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
         <v>50</v>
       </c>
@@ -1003,7 +996,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14">
+    <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
         <v>51</v>
       </c>
@@ -1011,7 +1004,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="14">
+    <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
         <v>56</v>
       </c>
@@ -1019,15 +1012,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="42">
+    <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="14">
+    <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
         <v>58</v>
       </c>
@@ -1035,7 +1028,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14">
+    <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
         <v>59</v>
       </c>
@@ -1043,7 +1036,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="14">
+    <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
         <v>60</v>
       </c>
@@ -1051,31 +1044,31 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="21">
-      <c r="A24" s="6" t="s">
+    <row r="24" spans="1:3">
+      <c r="A24" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="21">
-      <c r="A25" s="6" t="s">
+    <row r="25" spans="1:3">
+      <c r="A25" s="1" t="s">
         <v>67</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="14">
-      <c r="A26" s="3" t="s">
+    <row r="26" spans="1:3">
+      <c r="A26" s="1" t="s">
         <v>68</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="14">
+    <row r="27" spans="1:3">
       <c r="A27" s="1" t="s">
         <v>69</v>
       </c>
@@ -1083,60 +1076,60 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="14">
+    <row r="28" spans="1:3">
       <c r="A28" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="14">
+      <c r="C28" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="14">
-      <c r="A30" s="1"/>
-    </row>
-    <row r="31" spans="1:3" ht="13">
-      <c r="A31" s="3" t="s">
+    <row r="31" spans="1:3">
+      <c r="A31" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30">
-      <c r="A32" s="7" t="s">
+    <row r="32" spans="1:3">
+      <c r="A32" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="21">
-      <c r="A33" s="6" t="s">
+    <row r="33" spans="1:1">
+      <c r="A33" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="13">
-      <c r="A34" s="3" t="s">
+    <row r="34" spans="1:1">
+      <c r="A34" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="14">
+    <row r="35" spans="1:1">
       <c r="A35" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="14">
+    <row r="36" spans="1:1">
       <c r="A36" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="14">
+    <row r="37" spans="1:1">
       <c r="A37" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="13">
-      <c r="A38" s="3" t="s">
+    <row r="38" spans="1:1">
+      <c r="A38" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="14">
+    <row r="39" spans="1:1">
       <c r="A39" s="1" t="s">
         <v>78</v>
       </c>

</xml_diff>